<commit_message>
- started writting subsubsection ION Motion
</commit_message>
<xml_diff>
--- a/Illustrationen/Raw_Footage/Tabellen.xlsx
+++ b/Illustrationen/Raw_Footage/Tabellen.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="9525" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="9525" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FRDM-KL25Z Port Mapping" sheetId="1" r:id="rId1"/>
     <sheet name="LT3971 Überblick Daten" sheetId="2" r:id="rId2"/>
     <sheet name="LED Driver I2C Parameter" sheetId="3" r:id="rId3"/>
     <sheet name="LED Driver I2C Register Maps" sheetId="4" r:id="rId4"/>
+    <sheet name="ION Kommandos" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="252">
   <si>
     <t>J1 02</t>
   </si>
@@ -719,6 +720,60 @@
   </si>
   <si>
     <t>LED12–15 Selector</t>
+  </si>
+  <si>
+    <t>Adress (Dec)</t>
+  </si>
+  <si>
+    <t>Drive Forward Motor 1</t>
+  </si>
+  <si>
+    <t>Drive Backwards Motor 1</t>
+  </si>
+  <si>
+    <t>Drive Forward M2</t>
+  </si>
+  <si>
+    <t>Drive Backwards M2</t>
+  </si>
+  <si>
+    <t>Set Quadrature Encoder 1 Value</t>
+  </si>
+  <si>
+    <t>Kommando</t>
+  </si>
+  <si>
+    <t>Wertebereich</t>
+  </si>
+  <si>
+    <t>Set Quadrature Encoder 2 Value</t>
+  </si>
+  <si>
+    <t>Read Motor Currents</t>
+  </si>
+  <si>
+    <t>Buffered Drive M1 with signed Speed, Accel, Deccel and Position</t>
+  </si>
+  <si>
+    <t>Buffered Drive M2 with signed Speed, Accel, Deccel and Position</t>
+  </si>
+  <si>
+    <t>0… 127</t>
+  </si>
+  <si>
+    <t>0x00… 0xFF FF FF FF</t>
+  </si>
+  <si>
+    <t>2 / 2</t>
+  </si>
+  <si>
+    <t>0x00… 0xFF FF</t>
+  </si>
+  <si>
+    <t>4 / 4  / 4 / 4</t>
+  </si>
+  <si>
+    <t>Datenbytes</t>
   </si>
 </sst>
 </file>
@@ -806,7 +861,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -842,6 +897,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
@@ -2206,8 +2275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,4 +2444,167 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C8:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="59.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="20">
+        <v>0</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="E9" s="20">
+        <v>1</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="20">
+        <v>1</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" s="20">
+        <v>1</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="20">
+        <v>4</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="20">
+        <v>5</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="20">
+        <v>22</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="E13" s="20">
+        <v>4</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="20">
+        <v>23</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="E14" s="20">
+        <v>4</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="20">
+        <v>49</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="20">
+        <v>65</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="20">
+        <v>66</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- wrote section Evaluation der Komponenten - did some minor orthography corrections
</commit_message>
<xml_diff>
--- a/Illustrationen/Raw_Footage/Tabellen.xlsx
+++ b/Illustrationen/Raw_Footage/Tabellen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="9525" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="9525" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FRDM-KL25Z Port Mapping" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="LED Driver I2C Parameter" sheetId="3" r:id="rId3"/>
     <sheet name="LED Driver I2C Register Maps" sheetId="4" r:id="rId4"/>
     <sheet name="ION Kommandos" sheetId="5" r:id="rId5"/>
+    <sheet name="Trinamic" sheetId="6" r:id="rId6"/>
+    <sheet name="Pololu" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="279">
   <si>
     <t>J1 02</t>
   </si>
@@ -774,6 +776,87 @@
   </si>
   <si>
     <t>Datenbytes</t>
+  </si>
+  <si>
+    <t>Steuerung</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>QBL5704-116-04-042</t>
+  </si>
+  <si>
+    <t>TMCM-1630-2C</t>
+  </si>
+  <si>
+    <t>Nennspannung [V]</t>
+  </si>
+  <si>
+    <t>Nennstrom [A]</t>
+  </si>
+  <si>
+    <t>12… 55</t>
+  </si>
+  <si>
+    <t>max. Phasenstrom [A]</t>
+  </si>
+  <si>
+    <t>max. Motorenleistung [W]</t>
+  </si>
+  <si>
+    <t>Nenndrehzahl [1/min]</t>
+  </si>
+  <si>
+    <t>&lt; 100'000</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Nenndrehmoment [Nm]</t>
+  </si>
+  <si>
+    <t>max. Drehmoment [Nm]</t>
+  </si>
+  <si>
+    <t>Netzteil</t>
+  </si>
+  <si>
+    <t>HRP-600-36</t>
+  </si>
+  <si>
+    <t>Preis [CHF]</t>
+  </si>
+  <si>
+    <t>Motor Vereinzelung</t>
+  </si>
+  <si>
+    <t>Motor Verstellmechanik</t>
+  </si>
+  <si>
+    <t>Ansteuerung</t>
+  </si>
+  <si>
+    <t>RoboClaw 2x15A</t>
+  </si>
+  <si>
+    <t>99:1, 25Dx54L mm, HP</t>
+  </si>
+  <si>
+    <t>378:1, 25Dx58L mm, LP</t>
+  </si>
+  <si>
+    <t>6… 34</t>
+  </si>
+  <si>
+    <t>Anlauf Drehmoment [Nm]</t>
+  </si>
+  <si>
+    <t>NDR-120-12</t>
   </si>
 </sst>
 </file>
@@ -861,7 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -909,6 +992,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2450,7 +2551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C8:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -2607,4 +2708,319 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="27"/>
+      <c r="C3" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="7">
+        <v>36</v>
+      </c>
+      <c r="E5" s="7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6.67</v>
+      </c>
+      <c r="E6" s="7">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7">
+        <v>20.5</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" s="7">
+        <v>550</v>
+      </c>
+      <c r="D10" s="7">
+        <v>738</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="23">
+        <v>181.2</v>
+      </c>
+      <c r="D12" s="24">
+        <v>189.3</v>
+      </c>
+      <c r="E12" s="23">
+        <v>156.80000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="25"/>
+      <c r="D6" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>273</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" s="7">
+        <v>12</v>
+      </c>
+      <c r="F8" s="7">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="28">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G9" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="D10" s="28">
+        <v>30</v>
+      </c>
+      <c r="E10" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="7">
+        <v>100</v>
+      </c>
+      <c r="F12" s="7">
+        <v>14</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="D13" s="29">
+        <v>89.95</v>
+      </c>
+      <c r="E13" s="23">
+        <v>36.950000000000003</v>
+      </c>
+      <c r="F13" s="24">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="G13" s="23">
+        <v>40.950000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- wrote subsection Trinamic Motion Driver
</commit_message>
<xml_diff>
--- a/Illustrationen/Raw_Footage/Tabellen.xlsx
+++ b/Illustrationen/Raw_Footage/Tabellen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="9525" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="9525" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="FRDM-KL25Z Port Mapping" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="ION Kommandos" sheetId="5" r:id="rId5"/>
     <sheet name="Trinamic" sheetId="6" r:id="rId6"/>
     <sheet name="Pololu" sheetId="7" r:id="rId7"/>
+    <sheet name="Trinamic Motion Driver" sheetId="8" r:id="rId8"/>
+    <sheet name="Trinamic instructions" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="327">
   <si>
     <t>J1 02</t>
   </si>
@@ -857,6 +859,150 @@
   </si>
   <si>
     <t>NDR-120-12</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Reply address</t>
+  </si>
+  <si>
+    <t>Module address</t>
+  </si>
+  <si>
+    <t>Status (e.g. 100 means no error)</t>
+  </si>
+  <si>
+    <t>Command number</t>
+  </si>
+  <si>
+    <t>Value (MSB first!)</t>
+  </si>
+  <si>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t>Module adress</t>
+  </si>
+  <si>
+    <t>Type number</t>
+  </si>
+  <si>
+    <t>Motor or Bank number</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>ROR</t>
+  </si>
+  <si>
+    <t>ROL</t>
+  </si>
+  <si>
+    <t>MST</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>Rotate left</t>
+  </si>
+  <si>
+    <t>Rotate right</t>
+  </si>
+  <si>
+    <t>Motor stop</t>
+  </si>
+  <si>
+    <t>Move to position</t>
+  </si>
+  <si>
+    <t>Set axis parameter</t>
+  </si>
+  <si>
+    <t>Get axis parameter</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>GAP</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Axis Parameter</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Actual position</t>
+  </si>
+  <si>
+    <t>Set/get the position counter without moving the motor.</t>
+  </si>
+  <si>
+    <t>R / W</t>
+  </si>
+  <si>
+    <t>Set/get the max allowed motor current.</t>
+  </si>
+  <si>
+    <t>Max current</t>
+  </si>
+  <si>
+    <t>Acceleration parameter for ROL, ROR, and the velocity ramp of MVP.</t>
+  </si>
+  <si>
+    <t>Acceleration</t>
+  </si>
+  <si>
+    <t>Get actual motor current.</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Actual motor current</t>
+  </si>
+  <si>
+    <t>P parameter of current PID regulator.</t>
+  </si>
+  <si>
+    <t>I parameter of current PID regulator.</t>
+  </si>
+  <si>
+    <t>P parameter of velocity PID regulator.</t>
+  </si>
+  <si>
+    <t>I parameter of velocity PID regulator.</t>
+  </si>
+  <si>
+    <t>P parameter of position PID regulator.</t>
+  </si>
+  <si>
+    <t>P current PID</t>
+  </si>
+  <si>
+    <t>I current PID</t>
+  </si>
+  <si>
+    <t>P velocity PID</t>
+  </si>
+  <si>
+    <t>I velocity PID</t>
+  </si>
+  <si>
+    <t>P position PID</t>
   </si>
 </sst>
 </file>
@@ -944,7 +1090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1010,6 +1156,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2552,7 +2705,7 @@
   <dimension ref="C8:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C8" sqref="C8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,7 +3026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -3023,4 +3176,361 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:F10"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="10">
+        <v>4</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="62.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>303</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="D6" s="20">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="G8" s="6">
+        <v>11</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D9" s="20">
+        <v>4</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="G9" s="6">
+        <v>150</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="D10" s="20">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G10" s="6">
+        <v>172</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D11" s="20">
+        <v>6</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="G11" s="6">
+        <v>173</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="6">
+        <v>234</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="6">
+        <v>235</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="6">
+        <v>230</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- wrote subsection 4.1_Randbedingungen
</commit_message>
<xml_diff>
--- a/Illustrationen/Raw_Footage/Tabellen.xlsx
+++ b/Illustrationen/Raw_Footage/Tabellen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="9525" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22110" windowHeight="9525" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="FRDM-KL25Z Port Mapping" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Pololu" sheetId="7" r:id="rId7"/>
     <sheet name="Trinamic Motion Driver" sheetId="8" r:id="rId8"/>
     <sheet name="Trinamic instructions" sheetId="9" r:id="rId9"/>
+    <sheet name="Anforderungen Planting Robot" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="338">
   <si>
     <t>J1 02</t>
   </si>
@@ -1003,6 +1004,39 @@
   </si>
   <si>
     <t>P position PID</t>
+  </si>
+  <si>
+    <t>Lager</t>
+  </si>
+  <si>
+    <t>Bedingungen</t>
+  </si>
+  <si>
+    <t>Eigenschaft</t>
+  </si>
+  <si>
+    <t>10000 Nemacpas, nicht länger als 1 Tag</t>
+  </si>
+  <si>
+    <t>Speisung</t>
+  </si>
+  <si>
+    <t>230V Netzspannung, max. Leistungsaufnahme 2kW</t>
+  </si>
+  <si>
+    <t>Topferkennung</t>
+  </si>
+  <si>
+    <t>Setzprozess soll nur ausgeführt werden, wenn sich ein Topf auf dem Topfkranz befindet.</t>
+  </si>
+  <si>
+    <t>Topfkonfiguration</t>
+  </si>
+  <si>
+    <t>Pflicht: manuelle Konfiguration</t>
+  </si>
+  <si>
+    <t>Wunsch: automatische Konfiguration durch Topfgrössenerkennung</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1165,6 +1199,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
@@ -2338,6 +2373,72 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="80" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F9"/>
@@ -3310,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>